<commit_message>
updated employee models and setting up pilote and rq authorisations
</commit_message>
<xml_diff>
--- a/public/assets/extras/cadyst_liste_employee_modele.xlsx
+++ b/public/assets/extras/cadyst_liste_employee_modele.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\Documents\laravel\vacancy management\public\assets\extras\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\Documents\laravel\prd\public\assets\extras\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>ID</t>
   </si>
@@ -42,17 +42,10 @@
     <t>MOT DE PASSE</t>
   </si>
   <si>
-    <t>SERVICE</t>
-  </si>
-  <si>
     <t>TÉLÉPHONE</t>
   </si>
   <si>
     <t>MATRICULE</t>
-  </si>
-  <si>
-    <t>SOLDE
-VACANCE</t>
   </si>
   <si>
     <t>POSTE OCCUPÉ</t>
@@ -100,7 +93,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -109,9 +102,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -454,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -466,13 +456,12 @@
     <col min="2" max="2" width="16.25" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
     <col min="7" max="7" width="9.875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.25" customWidth="1"/>
-    <col min="11" max="11" width="12.5" customWidth="1"/>
-    <col min="12" max="12" width="9.625" customWidth="1"/>
+    <col min="8" max="8" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.25" customWidth="1"/>
+    <col min="10" max="10" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -498,19 +487,13 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -518,13 +501,11 @@
       <c r="E2" s="1"/>
       <c r="F2" s="2"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="1"/>
       <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -532,15 +513,14 @@
       <c r="E3" s="1"/>
       <c r="F3" s="2"/>
       <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="1"/>
       <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:I1" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:G1 H1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>